<commit_message>
corrects burndown chart for sprint 7
</commit_message>
<xml_diff>
--- a/SE202526/Management/Sprint7/burndown/Sprint7_Burndown.xlsx
+++ b/SE202526/Management/Sprint7/burndown/Sprint7_Burndown.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -2314,8 +2314,8 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="39266181"/>
-        <c:axId val="54236832"/>
+        <c:axId val="81583903"/>
+        <c:axId val="14262829"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -2642,11 +2642,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="39266181"/>
-        <c:axId val="54236832"/>
+        <c:axId val="81583903"/>
+        <c:axId val="14262829"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39266181"/>
+        <c:axId val="81583903"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2680,7 +2680,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54236832"/>
+        <c:crossAx val="14262829"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2688,7 +2688,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54236832"/>
+        <c:axId val="14262829"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -2767,7 +2767,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39266181"/>
+        <c:crossAx val="81583903"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2990,8 +2990,8 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="506259"/>
-        <c:axId val="80111504"/>
+        <c:axId val="1143508"/>
+        <c:axId val="43540127"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -3258,11 +3258,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="506259"/>
-        <c:axId val="80111504"/>
+        <c:axId val="1143508"/>
+        <c:axId val="43540127"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="506259"/>
+        <c:axId val="1143508"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3296,7 +3296,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80111504"/>
+        <c:crossAx val="43540127"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3304,7 +3304,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80111504"/>
+        <c:axId val="43540127"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -3383,7 +3383,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="506259"/>
+        <c:crossAx val="1143508"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3606,8 +3606,8 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="64810751"/>
-        <c:axId val="46547480"/>
+        <c:axId val="92590176"/>
+        <c:axId val="21364692"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -3874,11 +3874,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="64810751"/>
-        <c:axId val="46547480"/>
+        <c:axId val="92590176"/>
+        <c:axId val="21364692"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64810751"/>
+        <c:axId val="92590176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3912,7 +3912,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46547480"/>
+        <c:crossAx val="21364692"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3920,7 +3920,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46547480"/>
+        <c:axId val="21364692"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -3999,7 +3999,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64810751"/>
+        <c:crossAx val="92590176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4"/>
@@ -4200,8 +4200,8 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="44998661"/>
-        <c:axId val="86181157"/>
+        <c:axId val="72975097"/>
+        <c:axId val="5067932"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -4420,11 +4420,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="44998661"/>
-        <c:axId val="86181157"/>
+        <c:axId val="72975097"/>
+        <c:axId val="5067932"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44998661"/>
+        <c:axId val="72975097"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4458,7 +4458,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86181157"/>
+        <c:crossAx val="5067932"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4466,7 +4466,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86181157"/>
+        <c:axId val="5067932"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -4545,7 +4545,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44998661"/>
+        <c:crossAx val="72975097"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4"/>
@@ -4770,8 +4770,8 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="10745078"/>
-        <c:axId val="51749005"/>
+        <c:axId val="74736740"/>
+        <c:axId val="8744105"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -5038,11 +5038,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="10745078"/>
-        <c:axId val="51749005"/>
+        <c:axId val="74736740"/>
+        <c:axId val="8744105"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="10745078"/>
+        <c:axId val="74736740"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5076,7 +5076,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51749005"/>
+        <c:crossAx val="8744105"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5084,7 +5084,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51749005"/>
+        <c:axId val="8744105"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -5163,7 +5163,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10745078"/>
+        <c:crossAx val="74736740"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4"/>
@@ -5388,8 +5388,8 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="45650911"/>
-        <c:axId val="61313102"/>
+        <c:axId val="17447771"/>
+        <c:axId val="42943902"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -5656,11 +5656,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="45650911"/>
-        <c:axId val="61313102"/>
+        <c:axId val="17447771"/>
+        <c:axId val="42943902"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45650911"/>
+        <c:axId val="17447771"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5694,7 +5694,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61313102"/>
+        <c:crossAx val="42943902"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5702,7 +5702,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61313102"/>
+        <c:axId val="42943902"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="31"/>
@@ -5781,7 +5781,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45650911"/>
+        <c:crossAx val="17447771"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4"/>
@@ -5940,9 +5940,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Burndown Chart Sprint7'!$D$5:$K$5</c:f>
+              <c:f>'Burndown Chart Sprint7'!$D$5:$O$5</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>Dia 0</c:v>
                 </c:pt>
@@ -5966,16 +5966,28 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Dia 7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Dia 8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Dia 9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dia 10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dia 11</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart Sprint7'!$D$44:$K$44</c:f>
+              <c:f>'Burndown Chart Sprint7'!$D$44:$O$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -5998,6 +6010,18 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -6006,8 +6030,8 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="18409481"/>
-        <c:axId val="11547008"/>
+        <c:axId val="27270478"/>
+        <c:axId val="17840375"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -6077,9 +6101,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Burndown Chart Sprint7'!$D$5:$K$5</c:f>
+              <c:f>'Burndown Chart Sprint7'!$D$5:$O$5</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>Dia 0</c:v>
                 </c:pt>
@@ -6103,16 +6127,28 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Dia 7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Dia 8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Dia 9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dia 10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dia 11</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart Sprint7'!$D$45:$K$45</c:f>
+              <c:f>'Burndown Chart Sprint7'!$D$45:$O$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>69</c:v>
                 </c:pt>
@@ -6135,6 +6171,18 @@
                   <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>63.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>63.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>63.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>63.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>63.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -6201,9 +6249,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Burndown Chart Sprint7'!$D$5:$K$5</c:f>
+              <c:f>'Burndown Chart Sprint7'!$D$5:$O$5</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>Dia 0</c:v>
                 </c:pt>
@@ -6227,38 +6275,62 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Dia 7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Dia 8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Dia 9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dia 10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dia 11</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart Sprint7'!$D$46:$K$46</c:f>
+              <c:f>'Burndown Chart Sprint7'!$D$46:$O$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>15.6</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.3714285714286</c:v>
+                  <c:v>62.7272727272727</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.1428571428571</c:v>
+                  <c:v>56.4545454545455</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.91428571428572</c:v>
+                  <c:v>50.1818181818182</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.68571428571429</c:v>
+                  <c:v>43.9090909090909</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.45714285714286</c:v>
+                  <c:v>37.6363636363636</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.22857142857143</c:v>
+                  <c:v>31.3636363636364</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>25.0909090909091</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.8181818181818</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.5454545454545</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.27272727272727</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -6274,11 +6346,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="18409481"/>
-        <c:axId val="11547008"/>
+        <c:axId val="27270478"/>
+        <c:axId val="17840375"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="18409481"/>
+        <c:axId val="27270478"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6312,7 +6384,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11547008"/>
+        <c:crossAx val="17840375"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6320,10 +6392,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11547008"/>
+        <c:axId val="17840375"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="16"/>
+          <c:max val="70"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -6399,8 +6471,8 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18409481"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="27270478"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4"/>
         <c:minorUnit val="1.33333333333333"/>
@@ -6468,18 +6540,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>662400</xdr:colOff>
+      <xdr:colOff>662040</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>37080</xdr:rowOff>
+      <xdr:rowOff>36720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Chart 1"/>
+        <xdr:cNvPr id="1" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3403800" y="2685960"/>
-        <a:ext cx="9639360" cy="4885560"/>
+        <a:ext cx="9639000" cy="4885200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6503,18 +6575,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>14760</xdr:colOff>
+      <xdr:colOff>14400</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Chart 2"/>
+        <xdr:cNvPr id="2" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1155240" y="3543120"/>
-        <a:ext cx="9640080" cy="4885560"/>
+        <a:ext cx="9639720" cy="4885200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6538,18 +6610,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>348120</xdr:colOff>
+      <xdr:colOff>347760</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 3"/>
+        <xdr:cNvPr id="3" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1489320" y="7705800"/>
-        <a:ext cx="9639360" cy="4885560"/>
+        <a:ext cx="9639000" cy="4885200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6573,18 +6645,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>305280</xdr:colOff>
+      <xdr:colOff>304920</xdr:colOff>
       <xdr:row>81</xdr:row>
-      <xdr:rowOff>137880</xdr:rowOff>
+      <xdr:rowOff>137520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3846960" y="10025640"/>
-        <a:ext cx="9639000" cy="4885560"/>
+        <a:ext cx="9638640" cy="4885200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6608,18 +6680,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>348120</xdr:colOff>
+      <xdr:colOff>347760</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="5" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1489320" y="3362400"/>
-        <a:ext cx="9639360" cy="4885560"/>
+        <a:ext cx="9639000" cy="4885200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6643,18 +6715,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>890280</xdr:colOff>
+      <xdr:colOff>889920</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>181080</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 3"/>
+        <xdr:cNvPr id="6" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2969280" y="5652360"/>
-        <a:ext cx="9638640" cy="4885560"/>
+        <a:ext cx="9638280" cy="4885200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6678,18 +6750,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>348120</xdr:colOff>
+      <xdr:colOff>347760</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="7" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1489320" y="15381000"/>
-        <a:ext cx="9639360" cy="4885560"/>
+        <a:ext cx="9639000" cy="4885200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6900,8 +6972,8 @@
   </sheetPr>
   <dimension ref="B1:R1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O22" activeCellId="0" sqref="O22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8414,7 +8486,7 @@
   </sheetPr>
   <dimension ref="B1:M1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -9847,7 +9919,7 @@
   </sheetPr>
   <dimension ref="B1:P1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L45" activeCellId="0" sqref="L45"/>
     </sheetView>
   </sheetViews>
@@ -12271,7 +12343,7 @@
   </sheetPr>
   <dimension ref="A1:P988"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -15027,7 +15099,7 @@
   </sheetPr>
   <dimension ref="B1:P976"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -16549,7 +16621,7 @@
   </sheetPr>
   <dimension ref="B2:P37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O6" activeCellId="0" sqref="O6"/>
     </sheetView>
   </sheetViews>
@@ -17712,8 +17784,8 @@
   </sheetPr>
   <dimension ref="B1:T979"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T28" activeCellId="0" sqref="T28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C2" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E46" activeCellId="0" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18244,7 +18316,7 @@
         <f aca="false">SUM(E16:K16)</f>
         <v>0</v>
       </c>
-      <c r="S16" s="0" t="s">
+      <c r="S16" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -18278,7 +18350,7 @@
         <f aca="false">SUM(E17:K17)</f>
         <v>0</v>
       </c>
-      <c r="S17" s="0" t="s">
+      <c r="S17" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -18312,7 +18384,7 @@
         <f aca="false">SUM(E18:K18)</f>
         <v>0</v>
       </c>
-      <c r="S18" s="0" t="s">
+      <c r="S18" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -18346,7 +18418,7 @@
         <f aca="false">SUM(E19:K19)</f>
         <v>0</v>
       </c>
-      <c r="S19" s="0" t="s">
+      <c r="S19" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -18452,7 +18524,7 @@
         <f aca="false">SUM(E22:K22)</f>
         <v>0</v>
       </c>
-      <c r="S22" s="0" t="s">
+      <c r="S22" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -18486,7 +18558,7 @@
         <f aca="false">SUM(E23:K23)</f>
         <v>0</v>
       </c>
-      <c r="S23" s="0" t="s">
+      <c r="S23" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -18520,7 +18592,7 @@
         <f aca="false">SUM(E24:K24)</f>
         <v>0</v>
       </c>
-      <c r="S24" s="0" t="s">
+      <c r="S24" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -18554,7 +18626,7 @@
         <f aca="false">SUM(E25:K25)</f>
         <v>0</v>
       </c>
-      <c r="S25" s="0" t="s">
+      <c r="S25" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -18590,7 +18662,7 @@
         <f aca="false">SUM(E26:K26)</f>
         <v>0.5</v>
       </c>
-      <c r="S26" s="0" t="s">
+      <c r="S26" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -18626,7 +18698,7 @@
         <f aca="false">SUM(E27:K27)</f>
         <v>0.5</v>
       </c>
-      <c r="S27" s="0" t="s">
+      <c r="S27" s="1" t="s">
         <v>45</v>
       </c>
     </row>
@@ -18728,7 +18800,7 @@
         <f aca="false">SUM(E30:K30)</f>
         <v>0</v>
       </c>
-      <c r="S30" s="0" t="s">
+      <c r="S30" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -18762,7 +18834,7 @@
         <f aca="false">SUM(E31:K31)</f>
         <v>0</v>
       </c>
-      <c r="S31" s="0" t="s">
+      <c r="S31" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -18796,7 +18868,7 @@
         <f aca="false">SUM(E32:K32)</f>
         <v>0</v>
       </c>
-      <c r="S32" s="0" t="s">
+      <c r="S32" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -18830,7 +18902,7 @@
         <f aca="false">SUM(E33:K33)</f>
         <v>0</v>
       </c>
-      <c r="S33" s="0" t="s">
+      <c r="S33" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -18932,7 +19004,7 @@
         <f aca="false">SUM(E36:K36)</f>
         <v>0</v>
       </c>
-      <c r="S36" s="0" t="s">
+      <c r="S36" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -18966,7 +19038,7 @@
         <f aca="false">SUM(E37:K37)</f>
         <v>0</v>
       </c>
-      <c r="S37" s="0" t="s">
+      <c r="S37" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -19000,7 +19072,7 @@
         <f aca="false">SUM(E38:K38)</f>
         <v>0</v>
       </c>
-      <c r="S38" s="0" t="s">
+      <c r="S38" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -19034,7 +19106,7 @@
         <f aca="false">SUM(E39:K39)</f>
         <v>0</v>
       </c>
-      <c r="S39" s="0" t="s">
+      <c r="S39" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -19251,50 +19323,51 @@
       </c>
       <c r="C46" s="46"/>
       <c r="D46" s="47" t="n">
-        <v>15.6</v>
+        <f aca="false">D45</f>
+        <v>69</v>
       </c>
       <c r="E46" s="48" t="n">
-        <f aca="false">$D$46-($D$46/7*1)</f>
-        <v>13.3714285714286</v>
+        <f aca="false">$D$46-($D$46/11*1)</f>
+        <v>62.7272727272727</v>
       </c>
       <c r="F46" s="48" t="n">
-        <f aca="false">$D$46-($D$46/7*2)</f>
-        <v>11.1428571428571</v>
+        <f aca="false">$D$46-($D$46/11*2)</f>
+        <v>56.4545454545455</v>
       </c>
       <c r="G46" s="48" t="n">
-        <f aca="false">$D$46-($D$46/7*3)</f>
-        <v>8.91428571428572</v>
+        <f aca="false">$D$46-($D$46/11*3)</f>
+        <v>50.1818181818182</v>
       </c>
       <c r="H46" s="48" t="n">
-        <f aca="false">$D$46-($D$46/7*4)</f>
-        <v>6.68571428571429</v>
+        <f aca="false">$D$46-($D$46/11*4)</f>
+        <v>43.9090909090909</v>
       </c>
       <c r="I46" s="49" t="n">
-        <f aca="false">$D$46-($D$46/7*5)</f>
-        <v>4.45714285714286</v>
+        <f aca="false">$D$46-($D$46/11*5)</f>
+        <v>37.6363636363636</v>
       </c>
       <c r="J46" s="49" t="n">
-        <f aca="false">$D$46-($D$46/7*6)</f>
-        <v>2.22857142857143</v>
+        <f aca="false">$D$46-($D$46/11*6)</f>
+        <v>31.3636363636364</v>
       </c>
       <c r="K46" s="48" t="n">
-        <f aca="false">$D$46-($D$46/7*7)</f>
-        <v>0</v>
+        <f aca="false">$D$46-($D$46/11*7)</f>
+        <v>25.0909090909091</v>
       </c>
       <c r="L46" s="48" t="n">
-        <f aca="false">$D$46-($D$46/7*7)</f>
-        <v>0</v>
+        <f aca="false">$D$46-($D$46/11*8)</f>
+        <v>18.8181818181818</v>
       </c>
       <c r="M46" s="48" t="n">
-        <f aca="false">$D$46-($D$46/7*7)</f>
-        <v>0</v>
+        <f aca="false">$D$46-($D$46/11*9)</f>
+        <v>12.5454545454545</v>
       </c>
       <c r="N46" s="48" t="n">
-        <f aca="false">$D$46-($D$46/7*7)</f>
-        <v>0</v>
+        <f aca="false">$D$46-($D$46/11*10)</f>
+        <v>6.27272727272727</v>
       </c>
       <c r="O46" s="48" t="n">
-        <f aca="false">$D$46-($D$46/7*7)</f>
+        <f aca="false">$D$46-($D$46/11*11)</f>
         <v>0</v>
       </c>
     </row>
@@ -20279,12 +20352,12 @@
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B46:C46"/>
   </mergeCells>
-  <conditionalFormatting sqref="P6:P12">
+  <conditionalFormatting sqref="P6:P12 P13:P39 P40:P43">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>"DONE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P6:Q12">
+  <conditionalFormatting sqref="P6:Q12 P13:Q39 P40:Q43">
     <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"NOT ENOUGH WORK YET"</formula>
     </cfRule>
@@ -20295,7 +20368,7 @@
       <formula>"NOT STARTED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R6:R12 R14:R39">
+  <conditionalFormatting sqref="R6:R12 R14:R39 R13 R40:R43">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -20305,62 +20378,6 @@
         <color rgb="FFFFD666"/>
         <color rgb="FF00FF00"/>
       </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P13:P39">
-    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>"DONE"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P13:Q39">
-    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>"NOT ENOUGH WORK YET"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
-      <formula>"ERROR TO MUCH WORK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>"NOT STARTED"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R13">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="percentile" val="0.25"/>
-        <cfvo type="formula" val="0.5"/>
-        <color rgb="FF980000"/>
-        <color rgb="FFFFD666"/>
-        <color rgb="FF00FF00"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R40:R43">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="percentile" val="0.25"/>
-        <cfvo type="formula" val="0.5"/>
-        <color rgb="FF980000"/>
-        <color rgb="FFFFD666"/>
-        <color rgb="FF00FF00"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P40:P43">
-    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>"DONE"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P40:Q43">
-    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>"NOT ENOUGH WORK YET"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
-      <formula>"ERROR TO MUCH WORK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>"NOT STARTED"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>